<commit_message>
v3 launched to serve
</commit_message>
<xml_diff>
--- a/assets/uploads/booksExcelData/sample.xlsx
+++ b/assets/uploads/booksExcelData/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iamac\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bmb\assets\uploads\booksExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:40009_{84FDF643-2401-461D-8070-5CCF410A7E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1A99FBDD-6254-432E-940C-3D2A6547E1A0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627E2489-E1A1-471D-9652-E9FB11BCEA18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>isbn</t>
   </si>
@@ -85,7 +85,10 @@
     <t>asc</t>
   </si>
   <si>
-    <t>Available or N/A only</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Available or N/A (only Enter 1 from these)</t>
   </si>
 </sst>
 </file>
@@ -927,19 +930,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="P2" sqref="A1:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -977,14 +980,17 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1234567890</v>
       </c>
@@ -1019,13 +1025,16 @@
         <v>21</v>
       </c>
       <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
         <v>2</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>20</v>
       </c>
-      <c r="N2" t="s">
-        <v>21</v>
+      <c r="O2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>